<commit_message>
Made generic function instead of separate for diad1 and diad2 - iterative fitting if hit a warning
</commit_message>
<xml_diff>
--- a/docs/Examples/Diad_Fitting_Nov22nd2022/Fityk_results.xlsx
+++ b/docs/Examples/Diad_Fitting_Nov22nd2022/Fityk_results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\DiadFit_outer\docs\Examples\Diad_Fitting_Nov22nd2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BF5FBC-CEB8-4B91-A1AF-75722F174CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7940268D-240E-4C0A-ABDC-05E317F9BA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="34245" yWindow="2520" windowWidth="14400" windowHeight="7455" xr2:uid="{FF1FF9BC-1B90-4EFB-8E6E-B9863C148F5B}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10480" firstSheet="1" activeTab="1" xr2:uid="{FF1FF9BC-1B90-4EFB-8E6E-B9863C148F5B}"/>
   </bookViews>
   <sheets>
     <sheet name="112820_FULL" sheetId="1" r:id="rId1"/>
-    <sheet name="NEON" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
+    <sheet name="5thdec" sheetId="8" r:id="rId2"/>
+    <sheet name="NEON" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1074,7 +1075,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1090,6 +1091,12 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7326,11 +7333,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BDC9769-CDC1-424D-9AE4-8B7EF174E4CB}">
   <dimension ref="A1:X63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10199,78 +10206,78 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A39" s="3">
+    <row r="39" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="13">
         <v>44163</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="14">
         <v>0.9387847222222222</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="12">
         <v>1286.4811</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="12">
         <v>1389.3024</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="12">
         <f t="shared" si="4"/>
         <v>102.82130000000006</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="15">
         <f t="shared" si="5"/>
         <v>102.88301343893751</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="12">
         <v>1.79</v>
       </c>
-      <c r="I39" s="5">
+      <c r="I39" s="15">
         <v>1.7976616516113282</v>
       </c>
-      <c r="J39" s="5">
+      <c r="J39" s="15">
         <v>5.3420147268837259E-4</v>
       </c>
-      <c r="K39" s="6">
+      <c r="K39" s="16">
         <v>37</v>
       </c>
-      <c r="L39" s="9">
+      <c r="L39" s="17">
         <v>36.979999999999997</v>
       </c>
-      <c r="M39" s="7">
+      <c r="M39" s="18">
         <v>4.4444444444451392E-3</v>
       </c>
-      <c r="N39">
+      <c r="N39" s="12">
         <v>3.3450000000000001E-2</v>
       </c>
-      <c r="O39">
+      <c r="O39" s="12">
         <v>1123.4594</v>
       </c>
-      <c r="Q39">
+      <c r="Q39" s="12">
         <v>1453.7388000000001</v>
       </c>
-      <c r="R39">
+      <c r="R39" s="12">
         <f t="shared" si="6"/>
         <v>330.27940000000012</v>
       </c>
-      <c r="S39" s="9">
+      <c r="S39" s="17">
         <f t="shared" si="7"/>
         <v>330.47763400000008</v>
       </c>
-      <c r="T39" s="9">
+      <c r="T39" s="17">
         <v>1122.7762889999999</v>
       </c>
-      <c r="U39" s="9">
+      <c r="U39" s="17">
         <v>1225.7967639999999</v>
       </c>
-      <c r="V39" s="9">
+      <c r="V39" s="17">
         <v>1453.253923</v>
       </c>
-      <c r="W39" t="s">
+      <c r="W39" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="X39" t="s">
+      <c r="X39" s="12" t="s">
         <v>96</v>
       </c>
     </row>
@@ -11726,6 +11733,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05547686-82D0-477B-B94E-768A01BD3528}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8156891-BA79-4840-AC6F-FEF4D8CA7F3B}">
   <dimension ref="A1:BG78"/>
   <sheetViews>
@@ -16964,7 +16985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF7E02C-311D-4304-9009-D9F0B8179AF8}">
   <dimension ref="A1:V20"/>
   <sheetViews>

</xml_diff>